<commit_message>
Update E10 HR Data - Conditional Formatting.xlsx
</commit_message>
<xml_diff>
--- a/Exercise Files/Exercise 10/E10 HR Data - Conditional Formatting.xlsx
+++ b/Exercise Files/Exercise 10/E10 HR Data - Conditional Formatting.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f21e54c367d3358c/Documents/01 Work Files/05 SSIT/Online Courses/Advanced PivotTables/Exercise Files/Exercise 10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wayvy Technologies\Documents\GitHub\PivotTables\Exercise Files\Exercise 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{50E0B17D-4EEE-40B0-ADFD-53B45B9068E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3E09B68-30FD-444F-AEC8-85CC7E3EAB82}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76957275-0D92-4D19-9D2A-E5D95D697B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{960E11C6-F8C0-4296-BE1C-66F0D68FFF3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="1" r:id="rId1"/>
-    <sheet name="Conditional Formatting" sheetId="14" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId2"/>
+    <sheet name="Conditional Formatting" sheetId="14" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee Info'!$A$1:$C$100</definedName>
@@ -28,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="131">
   <si>
     <t>Employee ID</t>
   </si>
@@ -549,7 +550,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -557,7 +558,57 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -570,6 +621,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -645,11 +699,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Custom Style" table="0" count="5" xr9:uid="{20802757-926B-4C03-8B27-0A53E5554DB9}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="totalRow" dxfId="6"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="5"/>
-      <tableStyleElement type="pageFieldValues" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="11"/>
+      <tableStyleElement type="pageFieldValues" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -664,7 +718,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Department Info"/>
@@ -677,7 +731,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Job Info"/>
@@ -1954,457 +2008,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0CB1052F-B96A-4130-B0E0-BCEA0AB87490}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D14:E114" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="100">
-        <item x="22"/>
-        <item x="87"/>
-        <item x="31"/>
-        <item x="54"/>
-        <item x="56"/>
-        <item x="59"/>
-        <item x="82"/>
-        <item x="30"/>
-        <item x="92"/>
-        <item x="84"/>
-        <item x="18"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="6"/>
-        <item x="83"/>
-        <item x="19"/>
-        <item x="74"/>
-        <item x="67"/>
-        <item x="4"/>
-        <item x="86"/>
-        <item x="63"/>
-        <item x="12"/>
-        <item x="81"/>
-        <item x="20"/>
-        <item x="71"/>
-        <item x="65"/>
-        <item x="85"/>
-        <item x="70"/>
-        <item x="0"/>
-        <item x="10"/>
-        <item x="93"/>
-        <item x="37"/>
-        <item x="13"/>
-        <item x="69"/>
-        <item x="47"/>
-        <item x="95"/>
-        <item x="50"/>
-        <item x="14"/>
-        <item x="44"/>
-        <item x="43"/>
-        <item x="88"/>
-        <item x="60"/>
-        <item x="97"/>
-        <item x="32"/>
-        <item x="79"/>
-        <item x="29"/>
-        <item x="21"/>
-        <item x="98"/>
-        <item x="40"/>
-        <item x="49"/>
-        <item x="90"/>
-        <item x="1"/>
-        <item x="11"/>
-        <item x="38"/>
-        <item x="94"/>
-        <item x="57"/>
-        <item x="75"/>
-        <item x="80"/>
-        <item x="5"/>
-        <item x="26"/>
-        <item x="55"/>
-        <item x="48"/>
-        <item x="35"/>
-        <item x="7"/>
-        <item x="52"/>
-        <item x="36"/>
-        <item x="91"/>
-        <item x="89"/>
-        <item x="39"/>
-        <item x="8"/>
-        <item x="62"/>
-        <item x="23"/>
-        <item x="28"/>
-        <item x="64"/>
-        <item x="96"/>
-        <item x="34"/>
-        <item x="73"/>
-        <item x="51"/>
-        <item x="33"/>
-        <item x="61"/>
-        <item x="27"/>
-        <item x="17"/>
-        <item x="46"/>
-        <item x="58"/>
-        <item x="15"/>
-        <item x="72"/>
-        <item x="16"/>
-        <item x="76"/>
-        <item x="3"/>
-        <item x="77"/>
-        <item x="9"/>
-        <item x="66"/>
-        <item x="25"/>
-        <item x="24"/>
-        <item x="78"/>
-        <item x="53"/>
-        <item x="45"/>
-        <item x="68"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="44" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="100">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i>
-      <x v="47"/>
-    </i>
-    <i>
-      <x v="48"/>
-    </i>
-    <i>
-      <x v="49"/>
-    </i>
-    <i>
-      <x v="50"/>
-    </i>
-    <i>
-      <x v="51"/>
-    </i>
-    <i>
-      <x v="52"/>
-    </i>
-    <i>
-      <x v="53"/>
-    </i>
-    <i>
-      <x v="54"/>
-    </i>
-    <i>
-      <x v="55"/>
-    </i>
-    <i>
-      <x v="56"/>
-    </i>
-    <i>
-      <x v="57"/>
-    </i>
-    <i>
-      <x v="58"/>
-    </i>
-    <i>
-      <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
-    </i>
-    <i>
-      <x v="62"/>
-    </i>
-    <i>
-      <x v="63"/>
-    </i>
-    <i>
-      <x v="64"/>
-    </i>
-    <i>
-      <x v="65"/>
-    </i>
-    <i>
-      <x v="66"/>
-    </i>
-    <i>
-      <x v="67"/>
-    </i>
-    <i>
-      <x v="68"/>
-    </i>
-    <i>
-      <x v="69"/>
-    </i>
-    <i>
-      <x v="70"/>
-    </i>
-    <i>
-      <x v="71"/>
-    </i>
-    <i>
-      <x v="72"/>
-    </i>
-    <i>
-      <x v="73"/>
-    </i>
-    <i>
-      <x v="74"/>
-    </i>
-    <i>
-      <x v="75"/>
-    </i>
-    <i>
-      <x v="76"/>
-    </i>
-    <i>
-      <x v="77"/>
-    </i>
-    <i>
-      <x v="78"/>
-    </i>
-    <i>
-      <x v="79"/>
-    </i>
-    <i>
-      <x v="80"/>
-    </i>
-    <i>
-      <x v="81"/>
-    </i>
-    <i>
-      <x v="82"/>
-    </i>
-    <i>
-      <x v="83"/>
-    </i>
-    <i>
-      <x v="84"/>
-    </i>
-    <i>
-      <x v="85"/>
-    </i>
-    <i>
-      <x v="86"/>
-    </i>
-    <i>
-      <x v="87"/>
-    </i>
-    <i>
-      <x v="88"/>
-    </i>
-    <i>
-      <x v="89"/>
-    </i>
-    <i>
-      <x v="90"/>
-    </i>
-    <i>
-      <x v="91"/>
-    </i>
-    <i>
-      <x v="92"/>
-    </i>
-    <i>
-      <x v="93"/>
-    </i>
-    <i>
-      <x v="94"/>
-    </i>
-    <i>
-      <x v="95"/>
-    </i>
-    <i>
-      <x v="96"/>
-    </i>
-    <i>
-      <x v="97"/>
-    </i>
-    <i>
-      <x v="98"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Salary" fld="5" baseField="1" baseItem="2" numFmtId="42"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52BFFF8E-0061-4DC2-9102-9D6DA6732055}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B103" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
@@ -2870,10 +2473,24 @@
     <dataField name="Job Rating " fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
+  <conditionalFormats count="1">
+    <conditionalFormat scope="field" priority="9">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="0" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2886,7 +2503,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EC36FDE8-7C2F-4309-BC7F-D5321997CE9C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D3:F11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
@@ -2955,6 +2572,521 @@
     <dataField name="Sum of Salary" fld="5" baseField="3" baseItem="2" numFmtId="42"/>
     <dataField name="Average of Salary" fld="5" subtotal="average" baseField="3" baseItem="2" numFmtId="42"/>
   </dataFields>
+  <conditionalFormats count="4">
+    <conditionalFormat scope="field" priority="4">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="field" priority="3">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="3" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="field" priority="2">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="3" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat scope="field" priority="1">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="3" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0CB1052F-B96A-4130-B0E0-BCEA0AB87490}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D14:E114" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="100">
+        <item x="22"/>
+        <item x="87"/>
+        <item x="31"/>
+        <item x="54"/>
+        <item x="56"/>
+        <item x="59"/>
+        <item x="82"/>
+        <item x="30"/>
+        <item x="92"/>
+        <item x="84"/>
+        <item x="18"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="6"/>
+        <item x="83"/>
+        <item x="19"/>
+        <item x="74"/>
+        <item x="67"/>
+        <item x="4"/>
+        <item x="86"/>
+        <item x="63"/>
+        <item x="12"/>
+        <item x="81"/>
+        <item x="20"/>
+        <item x="71"/>
+        <item x="65"/>
+        <item x="85"/>
+        <item x="70"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="93"/>
+        <item x="37"/>
+        <item x="13"/>
+        <item x="69"/>
+        <item x="47"/>
+        <item x="95"/>
+        <item x="50"/>
+        <item x="14"/>
+        <item x="44"/>
+        <item x="43"/>
+        <item x="88"/>
+        <item x="60"/>
+        <item x="97"/>
+        <item x="32"/>
+        <item x="79"/>
+        <item x="29"/>
+        <item x="21"/>
+        <item x="98"/>
+        <item x="40"/>
+        <item x="49"/>
+        <item x="90"/>
+        <item x="1"/>
+        <item x="11"/>
+        <item x="38"/>
+        <item x="94"/>
+        <item x="57"/>
+        <item x="75"/>
+        <item x="80"/>
+        <item x="5"/>
+        <item x="26"/>
+        <item x="55"/>
+        <item x="48"/>
+        <item x="35"/>
+        <item x="7"/>
+        <item x="52"/>
+        <item x="36"/>
+        <item x="91"/>
+        <item x="89"/>
+        <item x="39"/>
+        <item x="8"/>
+        <item x="62"/>
+        <item x="23"/>
+        <item x="28"/>
+        <item x="64"/>
+        <item x="96"/>
+        <item x="34"/>
+        <item x="73"/>
+        <item x="51"/>
+        <item x="33"/>
+        <item x="61"/>
+        <item x="27"/>
+        <item x="17"/>
+        <item x="46"/>
+        <item x="58"/>
+        <item x="15"/>
+        <item x="72"/>
+        <item x="16"/>
+        <item x="76"/>
+        <item x="3"/>
+        <item x="77"/>
+        <item x="9"/>
+        <item x="66"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="78"/>
+        <item x="53"/>
+        <item x="45"/>
+        <item x="68"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="8">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="100">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="66"/>
+    </i>
+    <i>
+      <x v="67"/>
+    </i>
+    <i>
+      <x v="68"/>
+    </i>
+    <i>
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="75"/>
+    </i>
+    <i>
+      <x v="76"/>
+    </i>
+    <i>
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="78"/>
+    </i>
+    <i>
+      <x v="79"/>
+    </i>
+    <i>
+      <x v="80"/>
+    </i>
+    <i>
+      <x v="81"/>
+    </i>
+    <i>
+      <x v="82"/>
+    </i>
+    <i>
+      <x v="83"/>
+    </i>
+    <i>
+      <x v="84"/>
+    </i>
+    <i>
+      <x v="85"/>
+    </i>
+    <i>
+      <x v="86"/>
+    </i>
+    <i>
+      <x v="87"/>
+    </i>
+    <i>
+      <x v="88"/>
+    </i>
+    <i>
+      <x v="89"/>
+    </i>
+    <i>
+      <x v="90"/>
+    </i>
+    <i>
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="92"/>
+    </i>
+    <i>
+      <x v="93"/>
+    </i>
+    <i>
+      <x v="94"/>
+    </i>
+    <i>
+      <x v="95"/>
+    </i>
+    <i>
+      <x v="96"/>
+    </i>
+    <i>
+      <x v="97"/>
+    </i>
+    <i>
+      <x v="98"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Salary" fld="5" baseField="1" baseItem="2" numFmtId="42"/>
+  </dataFields>
+  <conditionalFormats count="1">
+    <conditionalFormat scope="field" type="all" priority="6">
+      <pivotAreas count="1">
+        <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="0" selected="0"/>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2976,19 +3108,37 @@
     <tableColumn id="3" xr3:uid="{CA98143F-2BDB-42FD-BC41-817FC0D04F36}" name="Gender"/>
     <tableColumn id="4" xr3:uid="{A1D24D7B-5420-4C14-98D4-ED4A6874AD3F}" name="Department"/>
     <tableColumn id="5" xr3:uid="{6912455C-0398-44C2-BF60-C4CFD7BB515C}" name="Manager"/>
-    <tableColumn id="6" xr3:uid="{EFABAA86-A780-4809-8095-CFC221E621BB}" name="Salary" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{EFABAA86-A780-4809-8095-CFC221E621BB}" name="Salary" dataDxfId="9" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{BE83895B-BC4C-4BDC-A9DA-0DC00422B3D8}" name="Job Type"/>
     <tableColumn id="9" xr3:uid="{7E616B03-35BF-4B3A-B0D0-C61556D6E9A8}" name="Job Rating"/>
-    <tableColumn id="8" xr3:uid="{5EBEFB9A-6064-43C4-B175-41F1F5C2BE6E}" name="Date Hired" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5EBEFB9A-6064-43C4-B175-41F1F5C2BE6E}" name="Date Hired" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E18752FF-BDF2-4FC5-8171-15F4E92005A6}" name="Table2" displayName="Table2" ref="A1:I2" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{E18752FF-BDF2-4FC5-8171-15F4E92005A6}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{5383441C-4382-4805-8AE4-2CEFD43B00CD}" name="Employee ID"/>
+    <tableColumn id="2" xr3:uid="{E033B43F-2270-40B1-B220-7887202AAB37}" name="Employee Name"/>
+    <tableColumn id="3" xr3:uid="{C708D2E4-9EE4-4D67-BA3B-C93F6F245BF3}" name="Gender"/>
+    <tableColumn id="4" xr3:uid="{8D97F051-9D5D-4D79-A35B-8F3ED317785E}" name="Department"/>
+    <tableColumn id="5" xr3:uid="{DCB29A70-8F46-4188-9B61-8B78883D39DE}" name="Manager"/>
+    <tableColumn id="6" xr3:uid="{CED47A10-D64A-4CA2-AE1D-961F0A3651F1}" name="Salary"/>
+    <tableColumn id="7" xr3:uid="{058D7804-0241-4842-88C6-60F2C27EDBB2}" name="Job Type"/>
+    <tableColumn id="8" xr3:uid="{63395D9E-2240-4E5B-8DEF-E8C80CDAF2A8}" name="Job Rating"/>
+    <tableColumn id="9" xr3:uid="{C482E6FF-6A6A-46BF-939C-DA22DA45FB1A}" name="Date Hired" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3026,7 +3176,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3132,7 +3282,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3274,7 +3424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3288,19 +3438,19 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="20.21875" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3329,7 +3479,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2100</v>
       </c>
@@ -3358,7 +3508,7 @@
         <v>40445</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2101</v>
       </c>
@@ -3387,7 +3537,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2102</v>
       </c>
@@ -3416,7 +3566,7 @@
         <v>43376</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2103</v>
       </c>
@@ -3445,7 +3595,7 @@
         <v>43168</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2104</v>
       </c>
@@ -3474,7 +3624,7 @@
         <v>40164</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2105</v>
       </c>
@@ -3503,7 +3653,7 @@
         <v>40511</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2106</v>
       </c>
@@ -3532,7 +3682,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2107</v>
       </c>
@@ -3561,7 +3711,7 @@
         <v>38555</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2108</v>
       </c>
@@ -3590,7 +3740,7 @@
         <v>42421</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2109</v>
       </c>
@@ -3619,7 +3769,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2110</v>
       </c>
@@ -3648,7 +3798,7 @@
         <v>42809</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2111</v>
       </c>
@@ -3677,7 +3827,7 @@
         <v>40378</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2112</v>
       </c>
@@ -3706,7 +3856,7 @@
         <v>40976</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2113</v>
       </c>
@@ -3735,7 +3885,7 @@
         <v>36845</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2114</v>
       </c>
@@ -3764,7 +3914,7 @@
         <v>42217</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2115</v>
       </c>
@@ -3793,7 +3943,7 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2116</v>
       </c>
@@ -3822,7 +3972,7 @@
         <v>36704</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2117</v>
       </c>
@@ -3851,7 +4001,7 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2118</v>
       </c>
@@ -3880,7 +4030,7 @@
         <v>41286</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2119</v>
       </c>
@@ -3909,7 +4059,7 @@
         <v>39319</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2120</v>
       </c>
@@ -3938,7 +4088,7 @@
         <v>40839</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2121</v>
       </c>
@@ -3967,7 +4117,7 @@
         <v>36754</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2122</v>
       </c>
@@ -3996,7 +4146,7 @@
         <v>38170</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2123</v>
       </c>
@@ -4025,7 +4175,7 @@
         <v>39164</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2124</v>
       </c>
@@ -4054,7 +4204,7 @@
         <v>42219</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2125</v>
       </c>
@@ -4083,7 +4233,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2126</v>
       </c>
@@ -4112,7 +4262,7 @@
         <v>41065</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2127</v>
       </c>
@@ -4141,7 +4291,7 @@
         <v>39692</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2128</v>
       </c>
@@ -4170,7 +4320,7 @@
         <v>42030</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2129</v>
       </c>
@@ -4199,7 +4349,7 @@
         <v>39499</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2130</v>
       </c>
@@ -4228,7 +4378,7 @@
         <v>43695</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2131</v>
       </c>
@@ -4257,7 +4407,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2132</v>
       </c>
@@ -4286,7 +4436,7 @@
         <v>36600</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2133</v>
       </c>
@@ -4315,7 +4465,7 @@
         <v>39803</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2134</v>
       </c>
@@ -4344,7 +4494,7 @@
         <v>40249</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2135</v>
       </c>
@@ -4373,7 +4523,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2136</v>
       </c>
@@ -4402,7 +4552,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2137</v>
       </c>
@@ -4431,7 +4581,7 @@
         <v>38241</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2138</v>
       </c>
@@ -4460,7 +4610,7 @@
         <v>40684</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2139</v>
       </c>
@@ -4489,7 +4639,7 @@
         <v>39996</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2140</v>
       </c>
@@ -4518,7 +4668,7 @@
         <v>37411</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2141</v>
       </c>
@@ -4547,7 +4697,7 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2142</v>
       </c>
@@ -4576,7 +4726,7 @@
         <v>43170</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2143</v>
       </c>
@@ -4605,7 +4755,7 @@
         <v>37292</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2144</v>
       </c>
@@ -4634,7 +4784,7 @@
         <v>37609</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2145</v>
       </c>
@@ -4663,7 +4813,7 @@
         <v>37094</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2146</v>
       </c>
@@ -4692,7 +4842,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2147</v>
       </c>
@@ -4721,7 +4871,7 @@
         <v>41517</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2148</v>
       </c>
@@ -4750,7 +4900,7 @@
         <v>38742</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2149</v>
       </c>
@@ -4779,7 +4929,7 @@
         <v>40047</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2150</v>
       </c>
@@ -4808,7 +4958,7 @@
         <v>39802</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2151</v>
       </c>
@@ -4837,7 +4987,7 @@
         <v>39616</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2152</v>
       </c>
@@ -4866,7 +5016,7 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2153</v>
       </c>
@@ -4895,7 +5045,7 @@
         <v>39019</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2154</v>
       </c>
@@ -4924,7 +5074,7 @@
         <v>41028</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2155</v>
       </c>
@@ -4953,7 +5103,7 @@
         <v>39768</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2156</v>
       </c>
@@ -4982,7 +5132,7 @@
         <v>41153</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2157</v>
       </c>
@@ -5011,7 +5161,7 @@
         <v>36847</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2158</v>
       </c>
@@ -5040,7 +5190,7 @@
         <v>37105</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2159</v>
       </c>
@@ -5069,7 +5219,7 @@
         <v>39744</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2160</v>
       </c>
@@ -5098,7 +5248,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2161</v>
       </c>
@@ -5127,7 +5277,7 @@
         <v>38401</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2162</v>
       </c>
@@ -5156,7 +5306,7 @@
         <v>37956</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2163</v>
       </c>
@@ -5185,7 +5335,7 @@
         <v>43907</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2164</v>
       </c>
@@ -5214,7 +5364,7 @@
         <v>43669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2165</v>
       </c>
@@ -5243,7 +5393,7 @@
         <v>39740</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2166</v>
       </c>
@@ -5272,7 +5422,7 @@
         <v>40408</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2167</v>
       </c>
@@ -5301,7 +5451,7 @@
         <v>38822</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2168</v>
       </c>
@@ -5330,7 +5480,7 @@
         <v>40083</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2169</v>
       </c>
@@ -5359,7 +5509,7 @@
         <v>41579</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2170</v>
       </c>
@@ -5388,7 +5538,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2171</v>
       </c>
@@ -5417,7 +5567,7 @@
         <v>41582</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2172</v>
       </c>
@@ -5446,7 +5596,7 @@
         <v>36663</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2173</v>
       </c>
@@ -5475,7 +5625,7 @@
         <v>37526</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2174</v>
       </c>
@@ -5504,7 +5654,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2175</v>
       </c>
@@ -5533,7 +5683,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2176</v>
       </c>
@@ -5562,7 +5712,7 @@
         <v>40107</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2177</v>
       </c>
@@ -5591,7 +5741,7 @@
         <v>39142</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2178</v>
       </c>
@@ -5620,7 +5770,7 @@
         <v>39165</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2179</v>
       </c>
@@ -5649,7 +5799,7 @@
         <v>42462</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2180</v>
       </c>
@@ -5678,7 +5828,7 @@
         <v>41654</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2181</v>
       </c>
@@ -5707,7 +5857,7 @@
         <v>43128</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2182</v>
       </c>
@@ -5736,7 +5886,7 @@
         <v>43381</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2183</v>
       </c>
@@ -5765,7 +5915,7 @@
         <v>41676</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2184</v>
       </c>
@@ -5794,7 +5944,7 @@
         <v>36651</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2185</v>
       </c>
@@ -5823,7 +5973,7 @@
         <v>42526</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2186</v>
       </c>
@@ -5852,7 +6002,7 @@
         <v>38565</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2187</v>
       </c>
@@ -5881,7 +6031,7 @@
         <v>37518</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2188</v>
       </c>
@@ -5910,7 +6060,7 @@
         <v>39656</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2189</v>
       </c>
@@ -5939,7 +6089,7 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2190</v>
       </c>
@@ -5968,7 +6118,7 @@
         <v>42528</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2191</v>
       </c>
@@ -5997,7 +6147,7 @@
         <v>38499</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2192</v>
       </c>
@@ -6026,7 +6176,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2193</v>
       </c>
@@ -6055,7 +6205,7 @@
         <v>38384</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2194</v>
       </c>
@@ -6084,7 +6234,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2195</v>
       </c>
@@ -6113,7 +6263,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2196</v>
       </c>
@@ -6142,7 +6292,7 @@
         <v>37442</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2197</v>
       </c>
@@ -6171,7 +6321,7 @@
         <v>38690</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2198</v>
       </c>
@@ -6209,25 +6359,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D32F2-88B1-42B1-9AEE-DA28855F1A43}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2">
+        <v>56146</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>38170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BB0522-9869-45F2-91D7-2DB9AFEA0E2A}">
   <dimension ref="A3:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6244,7 +6480,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -6261,7 +6497,7 @@
         <v>69913.055555555562</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -6278,7 +6514,7 @@
         <v>58320.166666666664</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -6295,7 +6531,7 @@
         <v>63516.823529411762</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -6312,7 +6548,7 @@
         <v>69485.307692307688</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -6329,7 +6565,7 @@
         <v>55287.666666666664</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -6346,7 +6582,7 @@
         <v>59283.888888888891</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -6363,7 +6599,7 @@
         <v>72643.555555555562</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -6380,7 +6616,7 @@
         <v>63896.222222222219</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -6388,7 +6624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -6396,7 +6632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -6410,7 +6646,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -6424,7 +6660,7 @@
         <v>56146</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -6438,7 +6674,7 @@
         <v>38206</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -6452,7 +6688,7 @@
         <v>27714</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -6466,7 +6702,7 @@
         <v>85983</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -6480,7 +6716,7 @@
         <v>79270</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -6494,7 +6730,7 @@
         <v>61939</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -6508,7 +6744,7 @@
         <v>94050</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -6522,7 +6758,7 @@
         <v>43304</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -6536,7 +6772,7 @@
         <v>70085</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -6550,7 +6786,7 @@
         <v>99568</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -6564,7 +6800,7 @@
         <v>47852</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -6578,7 +6814,7 @@
         <v>71398</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -6592,7 +6828,7 @@
         <v>86734</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -6606,7 +6842,7 @@
         <v>52320</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -6620,7 +6856,7 @@
         <v>82871</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -6634,7 +6870,7 @@
         <v>67560</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -6648,7 +6884,7 @@
         <v>84859</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -6662,7 +6898,7 @@
         <v>99248</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -6676,7 +6912,7 @@
         <v>66314</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -6690,7 +6926,7 @@
         <v>37471</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -6704,7 +6940,7 @@
         <v>32172</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -6718,7 +6954,7 @@
         <v>92006</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -6732,7 +6968,7 @@
         <v>63016</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -6746,7 +6982,7 @@
         <v>74344</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -6760,7 +6996,7 @@
         <v>57759</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -6774,7 +7010,7 @@
         <v>50945</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -6788,7 +7024,7 @@
         <v>44737</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -6802,7 +7038,7 @@
         <v>71067</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -6816,7 +7052,7 @@
         <v>86135</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -6830,7 +7066,7 @@
         <v>84304</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -6844,7 +7080,7 @@
         <v>90328</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -6858,7 +7094,7 @@
         <v>74903</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -6872,7 +7108,7 @@
         <v>32929</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -6886,7 +7122,7 @@
         <v>50831</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -6900,7 +7136,7 @@
         <v>62997</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -6914,7 +7150,7 @@
         <v>27723</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -6928,7 +7164,7 @@
         <v>70918</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -6942,7 +7178,7 @@
         <v>95191</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -6956,7 +7192,7 @@
         <v>47939</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>93</v>
       </c>
@@ -6970,7 +7206,7 @@
         <v>47199</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -6984,7 +7220,7 @@
         <v>79980</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>14</v>
       </c>
@@ -6998,7 +7234,7 @@
         <v>55197</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>41</v>
       </c>
@@ -7012,7 +7248,7 @@
         <v>33900</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -7026,7 +7262,7 @@
         <v>72568</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -7040,7 +7276,7 @@
         <v>56102</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -7054,7 +7290,7 @@
         <v>63662</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>83</v>
       </c>
@@ -7068,7 +7304,7 @@
         <v>51651</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -7082,7 +7318,7 @@
         <v>85288</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -7096,7 +7332,7 @@
         <v>59404</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>58</v>
       </c>
@@ -7110,7 +7346,7 @@
         <v>87377</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -7124,7 +7360,7 @@
         <v>33787</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -7138,7 +7374,7 @@
         <v>29587</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -7152,7 +7388,7 @@
         <v>26402</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -7166,7 +7402,7 @@
         <v>74201</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -7180,7 +7416,7 @@
         <v>95346</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -7194,7 +7430,7 @@
         <v>33778</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>92</v>
       </c>
@@ -7208,7 +7444,7 @@
         <v>76212</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -7222,7 +7458,7 @@
         <v>96503</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -7236,7 +7472,7 @@
         <v>60066</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -7250,7 +7486,7 @@
         <v>79169</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -7264,7 +7500,7 @@
         <v>50558</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -7278,7 +7514,7 @@
         <v>50441</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -7292,7 +7528,7 @@
         <v>61955</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>99</v>
       </c>
@@ -7306,7 +7542,7 @@
         <v>52949</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -7320,7 +7556,7 @@
         <v>92526</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -7334,7 +7570,7 @@
         <v>83169</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>54</v>
       </c>
@@ -7348,7 +7584,7 @@
         <v>58190</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -7362,7 +7598,7 @@
         <v>91367</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>64</v>
       </c>
@@ -7376,7 +7612,7 @@
         <v>78694</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>30</v>
       </c>
@@ -7390,7 +7626,7 @@
         <v>53638</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -7404,7 +7640,7 @@
         <v>62472</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>49</v>
       </c>
@@ -7418,7 +7654,7 @@
         <v>89126</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>61</v>
       </c>
@@ -7432,7 +7668,7 @@
         <v>61590</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -7446,7 +7682,7 @@
         <v>86357</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>75</v>
       </c>
@@ -7460,7 +7696,7 @@
         <v>40979</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -7474,7 +7710,7 @@
         <v>90608</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>79</v>
       </c>
@@ -7488,7 +7724,7 @@
         <v>91632</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -7502,7 +7738,7 @@
         <v>38413</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>80</v>
       </c>
@@ -7516,7 +7752,7 @@
         <v>29892</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -7530,7 +7766,7 @@
         <v>85414</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>69</v>
       </c>
@@ -7544,7 +7780,7 @@
         <v>36220</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>28</v>
       </c>
@@ -7558,7 +7794,7 @@
         <v>54102</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -7572,7 +7808,7 @@
         <v>97719</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>81</v>
       </c>
@@ -7586,7 +7822,7 @@
         <v>83237</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>56</v>
       </c>
@@ -7600,7 +7836,7 @@
         <v>56934</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -7614,7 +7850,7 @@
         <v>78859</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>71</v>
       </c>
@@ -7628,7 +7864,7 @@
         <v>87369</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -7642,7 +7878,7 @@
         <v>25504</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>126</v>
       </c>
@@ -7656,7 +7892,7 @@
         <v>40689</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D104" s="3" t="s">
         <v>80</v>
       </c>
@@ -7664,7 +7900,7 @@
         <v>78844</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D105" s="3" t="s">
         <v>12</v>
       </c>
@@ -7672,7 +7908,7 @@
         <v>27077</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D106" s="3" t="s">
         <v>69</v>
       </c>
@@ -7680,7 +7916,7 @@
         <v>51225</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D107" s="3" t="s">
         <v>28</v>
       </c>
@@ -7688,7 +7924,7 @@
         <v>55175</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D108" s="3" t="s">
         <v>27</v>
       </c>
@@ -7696,7 +7932,7 @@
         <v>87541</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D109" s="3" t="s">
         <v>81</v>
       </c>
@@ -7704,7 +7940,7 @@
         <v>56445</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D110" s="3" t="s">
         <v>56</v>
       </c>
@@ -7712,7 +7948,7 @@
         <v>64872</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D111" s="3" t="s">
         <v>48</v>
       </c>
@@ -7720,7 +7956,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D112" s="3" t="s">
         <v>71</v>
       </c>
@@ -7728,7 +7964,7 @@
         <v>48094</v>
       </c>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" s="3" t="s">
         <v>5</v>
       </c>
@@ -7736,7 +7972,7 @@
         <v>39748</v>
       </c>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" s="3" t="s">
         <v>126</v>
       </c>
@@ -7745,6 +7981,96 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting pivot="1" sqref="B4:B102">
+    <cfRule type="iconSet" priority="9">
+      <iconSet iconSet="3Arrows" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E15:E113">
+    <cfRule type="top10" dxfId="1" priority="6" rank="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E4:E10">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{07DE7BCF-7089-4255-99BC-BDCD76BF14B2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F4:F10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="F4:F10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="E4:E10">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F51194A3-B8BF-4DE4-AF74-A3645A762846}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{07DE7BCF-7089-4255-99BC-BDCD76BF14B2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E4:E10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" pivot="1">
+          <x14:cfRule type="dataBar" id="{F51194A3-B8BF-4DE4-AF74-A3645A762846}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E4:E10</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>